<commit_message>
Change the TVS diode for the buttons. Traced buttons net.
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/Estimation-Gastroscopy-CutController.xlsx
+++ b/DOCUMENTATION/Estimation-Gastroscopy-CutController.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Schematic design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCH &amp; PCB library</t>
   </si>
   <si>
     <t xml:space="preserve">Components placement</t>
@@ -237,10 +240,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -296,7 +299,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" s="3"/>
     </row>
@@ -320,7 +323,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -332,35 +335,47 @@
         <v>8</v>
       </c>
       <c r="C7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4" t="n">
-        <f aca="false">SUM(C2:C7)</f>
-        <v>17</v>
-      </c>
-      <c r="D8" s="4" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="4" t="n">
-        <f aca="false">C8/8</f>
-        <v>2.125</v>
+        <f aca="false">SUM(C2:C8)</f>
+        <v>31</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="1" t="n">
-        <f aca="false">_xlfn.CEILING.MATH(E1*C8)</f>
-        <v>11050</v>
+      <c r="C10" s="4" t="n">
+        <f aca="false">C9/8</f>
+        <v>3.875</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="1" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(E1*C9)</f>
+        <v>20150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>